<commit_message>
Object repository and screenshot
implemented standalone repository for object and action and implemented screenshot if testcase get failed
</commit_message>
<xml_diff>
--- a/testData/amazonloginobject.xlsx
+++ b/testData/amazonloginobject.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="login" sheetId="1" r:id="rId1"/>
+    <sheet name="objects" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -18,34 +18,34 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
-    <t>Click</t>
-  </si>
-  <si>
     <t>XPATH</t>
   </si>
   <si>
     <t>//android.widget.ImageButton[@content-desc="Main navigation, open"]</t>
   </si>
   <si>
-    <t>ClickBack</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
     <t>//android.widget.ImageView[@content-desc="eBay"]</t>
   </si>
   <si>
-    <t>validate</t>
-  </si>
-  <si>
     <t>ObjectType</t>
   </si>
   <si>
     <t>ObjectPath</t>
   </si>
   <si>
-    <t>Action</t>
+    <t>MenuButton</t>
+  </si>
+  <si>
+    <t>Device back</t>
+  </si>
+  <si>
+    <t>Title Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Object Description </t>
   </si>
 </sst>
 </file>
@@ -408,52 +408,53 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="67.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>